<commit_message>
Finished Air Events.. Ready to merge to main
</commit_message>
<xml_diff>
--- a/Config/Rules.xlsx
+++ b/Config/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CEEB4E-93CF-4B91-BB84-30F65CFA7609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D6315-C9EB-428A-96A2-25FA7FB7FEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1845" windowWidth="21600" windowHeight="11295" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3431,14 +3431,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;Bold&gt;r281 Special Travel Reference&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Refer to the Travel Table
- &lt;InlineUIContainer&gt;&lt;Button Content='t207' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and roll one die.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the appropriate line for the terrain type you occupy, read across to the Event References column and use the column listed for that die roll. This will produce a Travel Event Reference
-specified in the table.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r213 Rafting the Rivers&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You have the special option of using raft travel along the river instead of normal travel each day. When raft travel is available, you ride the raft until you get off by selecting a daily action other than raft travel; or when you roll 12 with two die after each day's travel. The latter represents the raft reaching a stopping point for lengthy loading, unloading, or dismantling.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;While on a raft, you travel on the river hexsides themselves. Your speed is either three hexsides per day downriver, or two hexsides per day upriver. 
@@ -3979,6 +3971,13 @@
       </rPr>
       <t>.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r281 Special Travel Reference&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Refer to the Travel Table
+ &lt;InlineUIContainer&gt;&lt;Button Content='t207' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and roll one die.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the appropriate line for the terrain type you occupy, read across to the Event References column and use the column listed for that die roll. This will produce a Travel Event Reference specified in the table.</t>
   </si>
 </sst>
 </file>
@@ -4361,8 +4360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,10 +4396,10 @@
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -4413,10 +4412,10 @@
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4461,18 +4460,18 @@
     </row>
     <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4501,34 +4500,34 @@
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4541,50 +4540,50 @@
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4840,7 +4839,7 @@
         <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4880,7 +4879,7 @@
         <v>29</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5040,7 +5039,7 @@
         <v>51</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5755,12 +5754,12 @@
         <v>322</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>404</v>
+        <v>435</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="45" x14ac:dyDescent="0.25">

</xml_diff>